<commit_message>
Added team name to testing document
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\checkers\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="4320" windowWidth="18705" windowHeight="7545" tabRatio="500"/>
   </bookViews>
@@ -106,9 +111,6 @@
     <t>fill in when doing cross-team or Freshman Seminar testing</t>
   </si>
   <si>
-    <t>Your team name as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers</t>
-  </si>
-  <si>
     <t>Tester initials; date; comments (required if test failed)</t>
   </si>
   <si>
@@ -117,6 +119,9 @@
 As tests are performed in each sprint, indicate Pass/Fail. The tester should add initials and a date in the comments column. If the test failed, the tester is required to add additional information about the failure. The status cell will color code based on the test results. The comments cell will color code when a test result exists but no information is entered.
 Save this test plan with a name formatted as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers.xslx.
 Submit this file per the instructions specified for the sprint submissions, cross-team testing, and Freshman Seminar testing.</t>
+  </si>
+  <si>
+    <t>2185-swen-261-02-b B++</t>
   </si>
 </sst>
 </file>
@@ -222,7 +227,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -271,197 +290,14 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -792,7 +628,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -806,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -814,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -841,7 +677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -868,19 +704,19 @@
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
@@ -3952,34 +3788,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C599 E2:E599 G2:G599">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D599">
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F599">
-    <cfRule type="expression" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H599">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>AND(ISBLANK(H2),G2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed problem in test document
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mightor\home\spring2019\rtk1357\Documents\checkers\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\checkers\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>Instructions</t>
   </si>
@@ -135,9 +134,6 @@
   </si>
   <si>
     <t>RK 3/2/19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK 3/2/19 </t>
   </si>
 </sst>
 </file>
@@ -625,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -840,7 +836,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>

</xml_diff>

<commit_message>
Made changes to Acceptance Test Plan. Greyed out sprint 1 tests
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -400,12 +400,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -449,7 +455,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -478,8 +484,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -490,28 +504,44 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -589,6 +619,66 @@
       </font>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -652,8 +742,8 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -699,555 +789,655 @@
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="C17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="19" t="s">
         <v>36</v>
       </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19" t="s">
         <v>37</v>
       </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19" t="s">
         <v>38</v>
       </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19" t="s">
         <v>39</v>
       </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19" t="s">
         <v>40</v>
       </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19" t="s">
         <v>41</v>
       </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19" t="s">
         <v>42</v>
       </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19" t="s">
         <v>43</v>
       </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="19" t="s">
         <v>45</v>
       </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="19" t="s">
         <v>47</v>
       </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19" t="s">
         <v>48</v>
       </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="15" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19" t="s">
         <v>49</v>
       </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="19" t="s">
         <v>51</v>
       </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19" t="s">
         <v>52</v>
       </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="15" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19" t="s">
         <v>53</v>
       </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="19" t="s">
         <v>55</v>
       </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="19" t="s">
         <v>57</v>
       </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19" t="s">
         <v>58</v>
       </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19" t="s">
         <v>59</v>
       </c>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="19" t="s">
         <v>61</v>
       </c>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19" t="s">
         <v>62</v>
       </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19" t="s">
         <v>63</v>
       </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
     </row>
     <row r="43" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="15" t="s">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19" t="s">
         <v>64</v>
       </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
     </row>
     <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="15" t="s">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19" t="s">
         <v>65</v>
       </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="15" t="s">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19" t="s">
         <v>66</v>
       </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
     </row>
     <row r="46" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19" t="s">
         <v>67</v>
       </c>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
     </row>
     <row r="47" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0"/>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19" t="s">
         <v>68</v>
       </c>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19" t="s">
         <v>69</v>
       </c>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0"/>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19" t="s">
         <v>70</v>
       </c>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
     </row>
     <row r="50" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0"/>
-      <c r="B50" s="15" t="s">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19" t="s">
         <v>71</v>
       </c>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
     </row>
     <row r="51" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="21" t="s">
         <v>73</v>
       </c>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
     </row>
     <row r="52" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="3" t="s">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20" t="s">
         <v>74</v>
       </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="3" t="s">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20" t="s">
         <v>75</v>
       </c>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
     </row>
     <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="3" t="s">
+      <c r="A54" s="20"/>
+      <c r="B54" s="20" t="s">
         <v>76</v>
       </c>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
     </row>
     <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="3" t="s">
+      <c r="A55" s="20"/>
+      <c r="B55" s="20" t="s">
         <v>77</v>
       </c>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
     </row>
     <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="3" t="s">
+      <c r="A56" s="20"/>
+      <c r="B56" s="20" t="s">
         <v>78</v>
       </c>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
     </row>
     <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="3" t="s">
+      <c r="A57" s="20"/>
+      <c r="B57" s="20" t="s">
         <v>79</v>
       </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
     </row>
     <row r="58" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="20" t="s">
         <v>81</v>
       </c>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="3" t="s">
+      <c r="A59" s="20"/>
+      <c r="B59" s="20" t="s">
         <v>82</v>
       </c>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
     </row>
     <row r="60" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="3" t="s">
+      <c r="A60" s="20"/>
+      <c r="B60" s="20" t="s">
         <v>83</v>
       </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
     </row>
     <row r="61" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="3" t="s">
+      <c r="A61" s="20"/>
+      <c r="B61" s="20" t="s">
         <v>84</v>
       </c>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="3" t="s">
+      <c r="A62" s="20"/>
+      <c r="B62" s="20" t="s">
         <v>85</v>
       </c>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
     </row>
     <row r="63" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="3" t="s">
+      <c r="A63" s="20"/>
+      <c r="B63" s="20" t="s">
         <v>86</v>
       </c>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C599 E2:E599 G2:G599">

</xml_diff>

<commit_message>
updated Acceptance test plan, but may need more updating
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doelc\Documents\GitHub\team-project-2185-swen-261-02-b-teamb\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF32B137-055C-43E9-B9F1-522E9A57D469}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Test Plan" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,165 +26,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
-  <si>
-    <t xml:space="preserve">Instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter your team name as specified in the cell below. When doing cross-team and Freshman Seminar acceptance testing, enter the name for the testing group.
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="90">
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Enter your team name as specified in the cell below. When doing cross-team and Freshman Seminar acceptance testing, enter the name for the testing group.
 Fill-in the Test Plan worksheet with all the remaining User Stories in your Product Backlog. As your user stories are refined, add the acceptance criteria for each user story. Use a separate worksheet to provide any specific test case data that the tester needs to use.
 As tests are performed in each sprint, indicate Pass/Fail. The tester should add initials and a date in the comments column. If the test failed, the tester is required to add additional information about the failure. The status cell will color code based on the test results. The comments cell will color code when a test result exists but no information is entered.
 Save this test plan with a name formatted as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers.xslx.
 Submit this file per the instructions specified for the sprint submissions, cross-team testing, and Freshman Seminar testing.</t>
   </si>
   <si>
-    <t xml:space="preserve">Team Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your team name as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Team Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fill in when doing cross-team or Freshman Seminar testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Story</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceptance Criterion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tester initials; date; comments (required if test failed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a Player I want to sign-in so that I can play a game of checkers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I have not yet signed in when I see the Home page then I must see a means to sign-in. (such as a link or button)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RF 2/26/19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am not signed-in when I do click on the sign-in link then I expect to be taken to the Signin page, with a means to enter a player name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that no one else is using my name when I enter my name in the sign-in form and click the Sign-in button then I expect system to reserve my name and navigate back to the Home page.</t>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Your team name as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers</t>
+  </si>
+  <si>
+    <t>Testing Team Name</t>
+  </si>
+  <si>
+    <t>fill in when doing cross-team or Freshman Seminar testing</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Acceptance Criterion</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Tester initials; date; comments (required if test failed)</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>As a Player I want to sign-in so that I can play a game of checkers.</t>
+  </si>
+  <si>
+    <t>Given that I have not yet signed in when I see the Home page then I must see a means to sign-in. (such as a link or button)</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>RF 2/26/19</t>
+  </si>
+  <si>
+    <t>Given that I am not signed-in when I do click on the sign-in link then I expect to be taken to the Signin page, with a means to enter a player name.</t>
+  </si>
+  <si>
+    <t>Given that no one else is using my name when I enter my name in the sign-in form and click the Sign-in button then I expect system to reserve my name and navigate back to the Home page.</t>
   </si>
   <si>
     <t xml:space="preserve">RF 3/2/19 </t>
   </si>
   <si>
-    <t xml:space="preserve">Given that no one else is using my name when I enter a name with a double quote (`"`) then I expect the system to reject this name and return the sign-in form.  (Note: double quote is not a valid character in a Player's name.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that someone else with my name has signed-in when I enter my name in the sign-in form then I expect the system to reject my sign-in and return the sign-in form.  I can then choose a different user name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I have signed in when I see the Home page then I must see a means to sign-out. (such as a link or button)  Thus the sign-in and sign-out links need to alternate and never been seen together or not at all.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am signed-in when I click on the sign-out link then I expect the system to sign me out, release my name for use by other users, and then return me to the Home page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am signed-in when I navigate to the Home page then I expect to see a list of all other signed-in players.  (NOTE: in the next story you will use this list to pick opponents for checkers games.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am not signed-in when I navigate to the Home page then I expect to see a message of how many players are signed-in but not a list of them (for privacy reasons).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a Player I want to start a game so that I can play checkers with an opponent.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I'm signed in when I view the Home page then I can start a game by selecting a player listed on the Home page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RK 3/2/19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that the player I selected isn't yet in a game when I select that player then the system will begin a checkers game and assign me as the starting (Red) player and my opponent as the White player.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that the player I selected is already in a game when I select that player then the system will return me to the Home page with an error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View from the Home page.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given a valid, initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given a valid, initial game board when I drag a piece to an open space then the piece should be droppable.  NOTE: In this Story the drop action should not do anything; piece movement will be the focus of future stories.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given a valid, initial game board when I view the board in the browser then my pieces are oriented on the bottom of the board grid just like I would see the board if I were playing in the physical world.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a player, I want to be able to 
+    <t>Given that no one else is using my name when I enter a name with a double quote (`"`) then I expect the system to reject this name and return the sign-in form.  (Note: double quote is not a valid character in a Player's name.)</t>
+  </si>
+  <si>
+    <t>Given that someone else with my name has signed-in when I enter my name in the sign-in form then I expect the system to reject my sign-in and return the sign-in form.  I can then choose a different user name.</t>
+  </si>
+  <si>
+    <t>Given that I have signed in when I see the Home page then I must see a means to sign-out. (such as a link or button)  Thus the sign-in and sign-out links need to alternate and never been seen together or not at all.</t>
+  </si>
+  <si>
+    <t>Given that I am signed-in when I click on the sign-out link then I expect the system to sign me out, release my name for use by other users, and then return me to the Home page.</t>
+  </si>
+  <si>
+    <t>Given that I am signed-in when I navigate to the Home page then I expect to see a list of all other signed-in players.  (NOTE: in the next story you will use this list to pick opponents for checkers games.)</t>
+  </si>
+  <si>
+    <t>Given that I am not signed-in when I navigate to the Home page then I expect to see a message of how many players are signed-in but not a list of them (for privacy reasons).</t>
+  </si>
+  <si>
+    <t>As a Player I want to start a game so that I can play checkers with an opponent.</t>
+  </si>
+  <si>
+    <t>Given that I'm signed in when I view the Home page then I can start a game by selecting a player listed on the Home page.</t>
+  </si>
+  <si>
+    <t>RK 3/2/19</t>
+  </si>
+  <si>
+    <t>Given that the player I selected isn't yet in a game when I select that player then the system will begin a checkers game and assign me as the starting (Red) player and my opponent as the White player.</t>
+  </si>
+  <si>
+    <t>Given that the player I selected is already in a game when I select that player then the system will return me to the Home page with an error message.</t>
+  </si>
+  <si>
+    <t>Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View from the Home page.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
+  </si>
+  <si>
+    <t>Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
+  </si>
+  <si>
+    <t>Given a valid, initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
+  </si>
+  <si>
+    <t>Given a valid, initial game board when I drag a piece to an open space then the piece should be droppable.  NOTE: In this Story the drop action should not do anything; piece movement will be the focus of future stories.</t>
+  </si>
+  <si>
+    <t>Given a valid, initial game board when I view the board in the browser then my pieces are oriented on the bottom of the board grid just like I would see the board if I were playing in the physical world.</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to 
 make moves when its my turn so 
 That I can progress the game.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn when I make a move then I expect the move to be 
+    <t>Given it is my turn when I make a move then I expect the move to be 
 Validated and logged by the server, but not shown to other players.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn and I've made a move when I press submit,
+    <t>Given it is my turn and I've made a move when I press submit,
  Then I expect the move to be finalized.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is not my turn when I try to move a piece then I 
+    <t>Given it is not my turn when I try to move a piece then I 
 Expect nothing to happen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is not my turn when I press submit, then I expect nothing to
+    <t>Given it is not my turn when I press submit, then I expect nothing to
  Happen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn and I haven’t made a move when I press submit then 
+    <t>Given it is my turn and I haven’t made a move when I press submit then 
 I expect that nothing will happen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn and I haven’t made a move when I press backup 
+    <t>Given it is my turn and I haven’t made a move when I press backup 
 Then I expect that nothing will happen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn and I’ve made an unfinalized move, when I press 
+    <t>Given it is my turn and I’ve made an unfinalized move, when I press 
 Backup then I expect that the move will be undone.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn when I finalize my move then my opponent 
+    <t>Given it is my turn when I finalize my move then my opponent 
 Should see the move and will then have their turn</t>
   </si>
   <si>
-    <t xml:space="preserve">As a player I want to move a single 
+    <t>As a player I want to move a single 
 piece across the board to an 
 Adjacent valid space.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given I’’m moving a piece for my turn when a vacant dark space is
+    <t>Given I’’m moving a piece for my turn when a vacant dark space is
  diagonally across from the piece I’m moving, then I expect that moving 
 To that space will be a valid move.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a player , I want to move a single 
+    <t>As a player , I want to move a single 
 piece over an opponent’s piece 
 diagonally forward and land on an 
 adjacent vacant dark square so that
@@ -187,32 +192,32 @@
 It is removed from the board.</t>
   </si>
   <si>
-    <t xml:space="preserve">Give I’m choosing a move when one of the other player’s pieces are 
+    <t>Give I’m choosing a move when one of the other player’s pieces are 
 diagonally adjacent to my piece and the spot diagonally behind their 
 Piece is clear, then jumping their piece with my piece is a valid move.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given that I just made a move when I jump one of my opponent’s pieces,
+    <t>Given that I just made a move when I jump one of my opponent’s pieces,
  Then I expect that piece is captured.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given that a jump move is available,when I want to submit my turn 
+    <t>Given that a jump move is available,when I want to submit my turn 
 Then I will be required to perform that jump.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a player, I want to move a single 
+    <t>As a player, I want to move a single 
 piece by jumping from vacant dark 
 square to vacant dark square so 
 that I capture an opponent’s piece 
 each jump.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it’s my turn, when I jump one of the other player’s pieces and 
+    <t>Given it’s my turn, when I jump one of the other player’s pieces and 
 another jump move is available, then I expect that the new jump move is
  Required.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn, when I jump one of the other players pieces and 
+    <t>Given it is my turn, when I jump one of the other players pieces and 
 another jump mov is availiable, then I expect to be able to perform that
  New jump.</t>
   </si>
@@ -222,7 +227,7 @@
  Validated. </t>
   </si>
   <si>
-    <t xml:space="preserve">As a player, I want to move my piece
+    <t>As a player, I want to move my piece
  to the king-row so that my turn may
  end, and my piece is promoted to 
 king by having the opponent place 
@@ -234,22 +239,22 @@
  After the turn has ended. </t>
   </si>
   <si>
-    <t xml:space="preserve">As a king piece I move and jump diagonally forward or backward so that I can move to vacant dark squares and claim opponent’s pieces.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given my piece is a king when I try to move it then I expect that 
+    <t>As a king piece I move and jump diagonally forward or backward so that I can move to vacant dark squares and claim opponent’s pieces.</t>
+  </si>
+  <si>
+    <t>Given my piece is a king when I try to move it then I expect that 
 Backwards moves are valid as well as forward moves.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given my piece is a king, when I try to backwards jump a piece, then I 
+    <t>Given my piece is a king, when I try to backwards jump a piece, then I 
 Expect that move to be validated.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given my piece is a king, when I try to multi jump backwards, then I 
+    <t>Given my piece is a king, when I try to multi jump backwards, then I 
 Expect all moves to be validated.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a player I want the game to end 
+    <t>As a player I want the game to end 
 So that I can play a different game.</t>
   </si>
   <si>
@@ -257,21 +262,21 @@
 Pieces then I should win the game. </t>
   </si>
   <si>
-    <t xml:space="preserve">Given a game is in progress when the last of my pieces are captured then
+    <t>Given a game is in progress when the last of my pieces are captured then
  I should lose the game.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given a game is in progress,it is my turn, and I haven’t made any 
+    <t>Given a game is in progress,it is my turn, and I haven’t made any 
 moves, when I cannot make a move with any of my pieces then I should 
 Lose the game.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given a game is in progress and it is my opponent’s turn when my 
+    <t>Given a game is in progress and it is my opponent’s turn when my 
 opponent cannot make a move with any of their pieces then I should win 
 The game.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given a game is in progress when I resign from the game then I should
+    <t>Given a game is in progress when I resign from the game then I should
  Lose the game.</t>
   </si>
   <si>
@@ -279,7 +284,7 @@
  Then I should win the game. </t>
   </si>
   <si>
-    <t xml:space="preserve">Given a game is in progress when a win/lose condition occurs and the
+    <t>Given a game is in progress when a win/lose condition occurs and the
  active player has submitted their turn then no further moves can be 
 Played and the board can be looked at in its final state.</t>
   </si>
@@ -288,11 +293,11 @@
  Should not be brought back to the game screen. </t>
   </si>
   <si>
-    <t xml:space="preserve">Given a game has ended when I’m looking at the final board state then I
+    <t>Given a game has ended when I’m looking at the final board state then I
  Should see an option to return to the home screen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given it is my turn when my opponent resigns the game and I
+    <t>Given it is my turn when my opponent resigns the game and I
  subsequently submit my turn, then the move is applied, the board is 
 Locked, and I win the game.</t>
   </si>
@@ -307,7 +312,7 @@
     <t xml:space="preserve">Given a game has two players when I join that game then I expect to view the game as a spectator </t>
   </si>
   <si>
-    <t xml:space="preserve">Given I am a spectator when I am in the game then I expect to not be able to affect the board.</t>
+    <t>Given I am a spectator when I am in the game then I expect to not be able to affect the board.</t>
   </si>
   <si>
     <t xml:space="preserve">Given I am a spectator when I am viewing a game then I expect to see a way to leave the game. </t>
@@ -316,44 +321,50 @@
     <t xml:space="preserve">Given I am a spectator when I am viewing a game then I expect the board to update when a player submits their turn. </t>
   </si>
   <si>
-    <t xml:space="preserve">Given I am a spectator when I view the game then I expect not to be dragged into a game with someone else.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I am a spectator when I leave a game then I expect to be redirected back to the home screen.</t>
+    <t>Given I am a spectator when I view the game then I expect not to be dragged into a game with someone else.</t>
+  </si>
+  <si>
+    <t>Given I am a spectator when I leave a game then I expect to be redirected back to the home screen.</t>
   </si>
   <si>
     <t xml:space="preserve">Given I am a player when I try to play a person spectating a different game then I expect to be given an error message. </t>
   </si>
   <si>
-    <t xml:space="preserve">As a user I want to replay a previously played game so that I can review the moves that were made (and otherwise enjoy it)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given at least one game has been finished when I’m browsing selection options on the hoe page then I should see a list of all finished games.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I’m playing a game when that game is finished then it should appear in a list of finished games.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given a game has been finished when I select it in a list of finished games then I should see the moves play out from beginning to end.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I am viewing a replay of a previous game when I hit the next button then the board should update to the next board state.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I view a replay of a previous game when I hit the previous button then the board should update to the previous board state.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I am viewing a replay of a previous game when I hit the exit button then I should be returned to the homepage.</t>
+    <t>As a user I want to replay a previously played game so that I can review the moves that were made (and otherwise enjoy it)</t>
+  </si>
+  <si>
+    <t>Given at least one game has been finished when I’m browsing selection options on the hoe page then I should see a list of all finished games.</t>
+  </si>
+  <si>
+    <t>Given I’m playing a game when that game is finished then it should appear in a list of finished games.</t>
+  </si>
+  <si>
+    <t>Given a game has been finished when I select it in a list of finished games then I should see the moves play out from beginning to end.</t>
+  </si>
+  <si>
+    <t>Given I am viewing a replay of a previous game when I hit the next button then the board should update to the next board state.</t>
+  </si>
+  <si>
+    <t>Given I view a replay of a previous game when I hit the previous button then the board should update to the previous board state.</t>
+  </si>
+  <si>
+    <t>Given I am viewing a replay of a previous game when I hit the exit button then I should be returned to the homepage.</t>
+  </si>
+  <si>
+    <t>SM 3/30/19</t>
+  </si>
+  <si>
+    <t>SW 4/13/19</t>
+  </si>
+  <si>
+    <t>SM 4/16/19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -362,30 +373,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -415,210 +410,151 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="medium"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
       </font>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -677,30 +613,338 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="106.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11"/>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="106.8984375" customWidth="1"/>
+    <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="220.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" ht="218.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -708,58 +952,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="4" width="10.89"/>
+    <col min="1" max="1" width="30" style="3" customWidth="1"/>
+    <col min="2" max="2" width="60" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9" style="3" customWidth="1"/>
+    <col min="4" max="4" width="60" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9" style="3" customWidth="1"/>
+    <col min="6" max="6" width="60" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" customWidth="1"/>
+    <col min="8" max="8" width="60" style="3" customWidth="1"/>
+    <col min="9" max="1025" width="10.8984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -785,7 +1021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -803,7 +1039,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -819,7 +1055,7 @@
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="8" t="s">
         <v>17</v>
@@ -835,7 +1071,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="8" t="s">
         <v>19</v>
@@ -851,7 +1087,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
@@ -867,7 +1103,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="8" t="s">
         <v>21</v>
@@ -883,7 +1119,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="8" t="s">
         <v>22</v>
@@ -899,7 +1135,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
         <v>23</v>
@@ -915,7 +1151,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
         <v>24</v>
@@ -931,7 +1167,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>25</v>
       </c>
@@ -949,7 +1185,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
@@ -965,7 +1201,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
         <v>29</v>
@@ -981,7 +1217,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="8" t="s">
         <v>30</v>
@@ -997,7 +1233,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>31</v>
@@ -1013,7 +1249,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="8" t="s">
         <v>32</v>
@@ -1029,7 +1265,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="8" t="s">
         <v>33</v>
@@ -1045,7 +1281,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
@@ -1061,7 +1297,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="9"/>
@@ -1071,419 +1307,586 @@
       <c r="G19" s="10"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-    </row>
-    <row r="24" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-    </row>
-    <row r="26" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-    </row>
-    <row r="27" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-    </row>
-    <row r="28" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-    </row>
-    <row r="29" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="156" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-    </row>
-    <row r="30" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-    </row>
-    <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="32" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="33" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-    </row>
-    <row r="34" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
     </row>
-    <row r="36" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-    </row>
-    <row r="37" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-    </row>
-    <row r="38" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
       <c r="B38" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-    </row>
-    <row r="40" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-    </row>
-    <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
       <c r="B41" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-    </row>
-    <row r="42" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
       <c r="B42" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-    </row>
-    <row r="43" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A43" s="19"/>
       <c r="B43" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-    </row>
-    <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-    </row>
-    <row r="45" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-    </row>
-    <row r="46" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
       <c r="B46" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-    </row>
-    <row r="47" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
       <c r="B48" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-    </row>
-    <row r="49" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
       <c r="B49" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-    </row>
-    <row r="50" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="19"/>
       <c r="B50" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-    </row>
-    <row r="51" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B51" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-    </row>
-    <row r="52" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="20"/>
       <c r="B52" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-    </row>
-    <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-    </row>
-    <row r="54" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-    </row>
-    <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-    </row>
-    <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
       <c r="B56" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-    </row>
-    <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-    </row>
-    <row r="58" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-    </row>
-    <row r="59" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
       <c r="B59" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-    </row>
-    <row r="60" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="20"/>
       <c r="B60" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-    </row>
-    <row r="61" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="20"/>
       <c r="B61" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-    </row>
-    <row r="62" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
       <c r="B62" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-    </row>
-    <row r="63" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="20"/>
       <c r="B63" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+      <c r="C63" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C599 E2:E599 G2:G599">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D599">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F599">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>AND(ISBLANK(F2),E2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H599">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>AND(ISBLANK(H2),G2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>AND(ISBLANK(H2),G2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C19 E2:E19 G2:G19" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C19 E2:E19 G2:G19" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>